<commit_message>
Updated the scope option of testng in pom.xml file
</commit_message>
<xml_diff>
--- a/target/test-classes/testData/TestSuite1.xlsx
+++ b/target/test-classes/testData/TestSuite1.xlsx
@@ -743,7 +743,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,7 +783,7 @@
         <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>